<commit_message>
Intégration de Dieppe dans Rouen
Signed-off-by: Guillaume Daudin <gdaudin@mac.com>
</commit_message>
<xml_diff>
--- a/Verified multipleformat sources/National par direction/AN/F12_1666 et 1667/1789-exportations-Dieppe_vérifié Silvia et LC.xlsx
+++ b/Verified multipleformat sources/National par direction/AN/F12_1666 et 1667/1789-exportations-Dieppe_vérifié Silvia et LC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loiccharles/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires Git/toflit18_data_GIT/Verified multipleformat sources/National par direction/AN/F12_1666 et 1667/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AF29D4-DA57-D44E-8895-417C818A22B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB506E3-9578-7243-A301-C166BDDE3AF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" tabRatio="984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="145">
   <si>
     <t>source</t>
   </si>
@@ -477,7 +477,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -502,6 +502,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -944,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AI77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1081,7 +1087,7 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>934</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
@@ -1121,14 +1127,14 @@
         <v>114</v>
       </c>
       <c r="O2" s="1"/>
-      <c r="P2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="P2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="R2" s="2">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="S2">
         <v>7600</v>
@@ -1154,7 +1160,7 @@
     </row>
     <row r="3" spans="1:35">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>934</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
@@ -1183,13 +1189,25 @@
       <c r="K3">
         <v>656</v>
       </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="2">
+        <v>29</v>
+      </c>
       <c r="S3">
         <v>656</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>934</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
@@ -1218,13 +1236,25 @@
       <c r="K4">
         <v>8064</v>
       </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="2">
+        <v>29</v>
+      </c>
       <c r="S4">
         <v>8064</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>934</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
@@ -1253,13 +1283,25 @@
       <c r="K5">
         <v>9500</v>
       </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="2">
+        <v>29</v>
+      </c>
       <c r="S5">
         <v>9500</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>934</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -1288,13 +1330,25 @@
       <c r="K6">
         <v>4560</v>
       </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="2">
+        <v>29</v>
+      </c>
       <c r="S6">
         <v>4560</v>
       </c>
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>934</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
@@ -1323,19 +1377,31 @@
       <c r="K7">
         <v>144</v>
       </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
       <c r="M7" s="6">
         <v>12</v>
       </c>
       <c r="N7" t="s">
         <v>128</v>
       </c>
+      <c r="P7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" s="2">
+        <v>29</v>
+      </c>
       <c r="S7">
         <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:35">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>934</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>35</v>
@@ -1364,19 +1430,31 @@
       <c r="K8">
         <v>4800</v>
       </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
       <c r="M8" s="6">
         <v>100</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>125</v>
       </c>
+      <c r="P8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8" s="2">
+        <v>29</v>
+      </c>
       <c r="S8">
         <v>4800</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>934</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>35</v>
@@ -1405,13 +1483,25 @@
       <c r="K9">
         <v>15807</v>
       </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R9" s="2">
+        <v>29</v>
+      </c>
       <c r="S9">
         <v>15807</v>
       </c>
     </row>
     <row r="10" spans="1:35">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>934</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
@@ -1440,19 +1530,31 @@
       <c r="K10">
         <v>178</v>
       </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
       <c r="M10" s="6">
         <v>178</v>
       </c>
       <c r="N10" t="s">
         <v>115</v>
       </c>
+      <c r="P10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="2">
+        <v>29</v>
+      </c>
       <c r="S10">
         <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:35">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>934</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>35</v>
@@ -1481,19 +1583,31 @@
       <c r="K11">
         <v>1500</v>
       </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
       <c r="M11" s="6">
         <v>700</v>
       </c>
       <c r="N11" t="s">
         <v>115</v>
       </c>
+      <c r="P11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" s="2">
+        <v>29</v>
+      </c>
       <c r="S11">
         <v>1500</v>
       </c>
     </row>
     <row r="12" spans="1:35">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>934</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
@@ -1522,19 +1636,31 @@
       <c r="K12">
         <v>2700</v>
       </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
       <c r="M12" s="6">
         <v>3</v>
       </c>
       <c r="N12" t="s">
         <v>115</v>
       </c>
+      <c r="P12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R12" s="2">
+        <v>29</v>
+      </c>
       <c r="S12">
         <v>2700</v>
       </c>
     </row>
     <row r="13" spans="1:35">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>934</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>35</v>
@@ -1563,19 +1689,31 @@
       <c r="K13">
         <v>6624</v>
       </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
       <c r="M13" s="6">
         <v>207</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>116</v>
       </c>
+      <c r="P13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="2">
+        <v>29</v>
+      </c>
       <c r="S13">
         <v>6624</v>
       </c>
     </row>
     <row r="14" spans="1:35">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>934</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -1604,19 +1742,31 @@
       <c r="K14">
         <v>10880</v>
       </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
       <c r="M14" s="6">
         <v>272</v>
       </c>
       <c r="N14" s="7" t="s">
         <v>116</v>
       </c>
+      <c r="P14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="2">
+        <v>29</v>
+      </c>
       <c r="S14">
         <v>10880</v>
       </c>
     </row>
     <row r="15" spans="1:35">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>934</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
@@ -1645,19 +1795,31 @@
       <c r="K15">
         <v>4160</v>
       </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
       <c r="M15" s="6">
         <v>260</v>
       </c>
       <c r="N15" s="7" t="s">
         <v>116</v>
       </c>
+      <c r="P15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" s="2">
+        <v>29</v>
+      </c>
       <c r="S15">
         <v>4160</v>
       </c>
     </row>
     <row r="16" spans="1:35">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>934</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>35</v>
@@ -1686,19 +1848,31 @@
       <c r="K16">
         <v>820</v>
       </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
       <c r="M16" s="6">
         <v>410</v>
       </c>
       <c r="N16" t="s">
         <v>115</v>
       </c>
+      <c r="P16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R16" s="2">
+        <v>29</v>
+      </c>
       <c r="S16">
         <v>820</v>
       </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>934</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
@@ -1726,6 +1900,9 @@
       </c>
       <c r="K17">
         <v>3840</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
       </c>
       <c r="M17" s="8">
         <f>17+224/288</f>
@@ -1734,13 +1911,22 @@
       <c r="N17" s="7" t="s">
         <v>129</v>
       </c>
+      <c r="P17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="2">
+        <v>29</v>
+      </c>
       <c r="S17">
         <v>3840</v>
       </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>934</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
@@ -1769,13 +1955,25 @@
       <c r="K18">
         <v>488</v>
       </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="2">
+        <v>29</v>
+      </c>
       <c r="S18">
         <v>36508</v>
       </c>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>934</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>35</v>
@@ -1804,13 +2002,25 @@
       <c r="K19">
         <v>36020</v>
       </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R19" s="2">
+        <v>29</v>
+      </c>
       <c r="S19">
         <v>36508</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>934</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>35</v>
@@ -1839,13 +2049,25 @@
       <c r="K20">
         <v>14542</v>
       </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R20" s="2">
+        <v>29</v>
+      </c>
       <c r="S20">
         <v>14542</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>934</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>35</v>
@@ -1874,19 +2096,31 @@
       <c r="K21">
         <v>640</v>
       </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
       <c r="M21" s="6">
         <v>291</v>
       </c>
       <c r="N21" s="7" t="s">
         <v>116</v>
       </c>
+      <c r="P21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R21" s="2">
+        <v>29</v>
+      </c>
       <c r="S21">
         <v>640</v>
       </c>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>934</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>35</v>
@@ -1915,13 +2149,25 @@
       <c r="K22">
         <v>1533</v>
       </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R22" s="2">
+        <v>29</v>
+      </c>
       <c r="S22">
         <v>1533</v>
       </c>
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>934</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>35</v>
@@ -1950,13 +2196,25 @@
       <c r="K23">
         <v>401</v>
       </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="2">
+        <v>29</v>
+      </c>
       <c r="S23">
         <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>934</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>35</v>
@@ -1985,19 +2243,31 @@
       <c r="K24">
         <v>240</v>
       </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
       <c r="M24" s="6">
         <v>7.5</v>
       </c>
       <c r="N24" s="7" t="s">
         <v>115</v>
       </c>
+      <c r="P24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R24" s="2">
+        <v>29</v>
+      </c>
       <c r="S24">
         <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>934</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>35</v>
@@ -2026,19 +2296,31 @@
       <c r="K25">
         <v>1858</v>
       </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
       <c r="M25" s="6">
         <v>782</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>116</v>
       </c>
+      <c r="P25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R25" s="2">
+        <v>29</v>
+      </c>
       <c r="S25">
         <v>1858</v>
       </c>
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>934</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
@@ -2067,12 +2349,24 @@
       <c r="K26">
         <v>4800</v>
       </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
       <c r="M26" s="6">
         <v>450</v>
       </c>
       <c r="N26" s="7" t="s">
         <v>116</v>
       </c>
+      <c r="P26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R26" s="2">
+        <v>29</v>
+      </c>
       <c r="S26">
         <v>4800</v>
       </c>
@@ -2082,7 +2376,7 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>934</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>35</v>
@@ -2111,19 +2405,31 @@
       <c r="K27">
         <v>300</v>
       </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
       <c r="M27" s="6">
         <v>50</v>
       </c>
       <c r="N27" t="s">
         <v>115</v>
       </c>
+      <c r="P27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R27" s="2">
+        <v>29</v>
+      </c>
       <c r="S27">
         <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>934</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>35</v>
@@ -2152,13 +2458,25 @@
       <c r="K28">
         <v>205</v>
       </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R28" s="2">
+        <v>29</v>
+      </c>
       <c r="S28">
         <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>934</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
@@ -2187,19 +2505,31 @@
       <c r="K29">
         <v>680</v>
       </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
       <c r="M29" s="6">
         <v>3400</v>
       </c>
       <c r="N29" t="s">
         <v>115</v>
       </c>
+      <c r="P29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R29" s="2">
+        <v>29</v>
+      </c>
       <c r="S29">
         <v>680</v>
       </c>
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>934</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>35</v>
@@ -2228,19 +2558,31 @@
       <c r="K30">
         <v>450</v>
       </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
       <c r="M30" s="6">
         <v>1075</v>
       </c>
       <c r="N30" t="s">
         <v>115</v>
       </c>
+      <c r="P30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R30" s="2">
+        <v>29</v>
+      </c>
       <c r="S30">
         <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>934</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>35</v>
@@ -2269,19 +2611,31 @@
       <c r="K31">
         <v>2543</v>
       </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
       <c r="M31">
         <v>10182</v>
       </c>
       <c r="N31" s="7" t="s">
         <v>115</v>
       </c>
+      <c r="P31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R31" s="2">
+        <v>29</v>
+      </c>
       <c r="S31">
         <v>2543</v>
       </c>
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>934</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>35</v>
@@ -2310,13 +2664,25 @@
       <c r="K32">
         <v>856</v>
       </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R32" s="2">
+        <v>29</v>
+      </c>
       <c r="S32">
         <v>856</v>
       </c>
     </row>
     <row r="33" spans="1:25">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>934</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>35</v>
@@ -2345,19 +2711,31 @@
       <c r="K33">
         <v>210</v>
       </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
       <c r="M33">
         <v>699</v>
       </c>
       <c r="N33" t="s">
         <v>115</v>
       </c>
+      <c r="P33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R33" s="2">
+        <v>29</v>
+      </c>
       <c r="S33">
         <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>934</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -2386,19 +2764,31 @@
       <c r="K34">
         <v>38500</v>
       </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
       <c r="M34" s="6">
         <v>10853</v>
       </c>
       <c r="N34" t="s">
         <v>115</v>
       </c>
+      <c r="P34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R34" s="2">
+        <v>29</v>
+      </c>
       <c r="S34">
         <v>38500</v>
       </c>
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>934</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>35</v>
@@ -2427,13 +2817,25 @@
       <c r="K35" s="6">
         <v>169</v>
       </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R35" s="2">
+        <v>29</v>
+      </c>
       <c r="S35">
         <v>1723</v>
       </c>
     </row>
     <row r="36" spans="1:25">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>934</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>35</v>
@@ -2462,13 +2864,25 @@
       <c r="K36" s="6">
         <v>1256</v>
       </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R36" s="2">
+        <v>29</v>
+      </c>
       <c r="S36">
         <v>1723</v>
       </c>
     </row>
     <row r="37" spans="1:25">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>934</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>35</v>
@@ -2497,13 +2911,25 @@
       <c r="K37" s="6">
         <v>176</v>
       </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R37" s="2">
+        <v>29</v>
+      </c>
       <c r="S37">
         <v>1723</v>
       </c>
     </row>
     <row r="38" spans="1:25">
       <c r="A38" s="1">
-        <v>37</v>
+        <v>934</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>35</v>
@@ -2532,13 +2958,25 @@
       <c r="K38" s="6">
         <v>185</v>
       </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R38" s="2">
+        <v>29</v>
+      </c>
       <c r="S38">
         <v>1723</v>
       </c>
     </row>
     <row r="39" spans="1:25">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>934</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>35</v>
@@ -2567,13 +3005,25 @@
       <c r="K39" s="6">
         <v>106</v>
       </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R39" s="2">
+        <v>29</v>
+      </c>
       <c r="S39">
         <v>1723</v>
       </c>
     </row>
     <row r="40" spans="1:25">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>934</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>35</v>
@@ -2602,13 +3052,25 @@
       <c r="K40" s="6">
         <v>25385</v>
       </c>
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R40" s="2">
+        <v>29</v>
+      </c>
       <c r="S40">
         <v>25385</v>
       </c>
     </row>
     <row r="41" spans="1:25">
       <c r="A41" s="1">
-        <v>40</v>
+        <v>934</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>35</v>
@@ -2637,13 +3099,25 @@
       <c r="K41" s="6">
         <v>2069</v>
       </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R41" s="2">
+        <v>29</v>
+      </c>
       <c r="S41">
         <v>2069</v>
       </c>
     </row>
     <row r="42" spans="1:25">
       <c r="A42" s="1">
-        <v>41</v>
+        <v>934</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>35</v>
@@ -2671,6 +3145,9 @@
       </c>
       <c r="K42" s="6">
         <v>6684</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0</v>
       </c>
       <c r="M42" s="13">
         <f>139+(2/24)</f>
@@ -2679,6 +3156,15 @@
       <c r="N42" s="14" t="s">
         <v>142</v>
       </c>
+      <c r="P42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R42" s="4">
+        <v>30</v>
+      </c>
       <c r="S42">
         <v>6684</v>
       </c>
@@ -2688,7 +3174,7 @@
     </row>
     <row r="43" spans="1:25">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>934</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>35</v>
@@ -2717,19 +3203,31 @@
       <c r="K43" s="6">
         <v>1500</v>
       </c>
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
       <c r="M43" s="6">
         <v>50000</v>
       </c>
       <c r="N43" t="s">
         <v>114</v>
       </c>
+      <c r="P43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R43" s="4">
+        <v>30</v>
+      </c>
       <c r="S43">
         <v>1500</v>
       </c>
     </row>
     <row r="44" spans="1:25">
       <c r="A44" s="1">
-        <v>43</v>
+        <v>934</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>35</v>
@@ -2758,13 +3256,25 @@
       <c r="K44" s="6">
         <v>273</v>
       </c>
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R44" s="4">
+        <v>30</v>
+      </c>
       <c r="S44">
         <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="1">
-        <v>44</v>
+        <v>934</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>35</v>
@@ -2793,13 +3303,25 @@
       <c r="K45" s="8">
         <v>197</v>
       </c>
+      <c r="L45" s="1">
+        <v>0</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R45" s="4">
+        <v>30</v>
+      </c>
       <c r="Y45" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:25">
       <c r="A46" s="1">
-        <v>45</v>
+        <v>934</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>35</v>
@@ -2828,13 +3350,25 @@
       <c r="K46" s="6">
         <v>150</v>
       </c>
+      <c r="L46" s="1">
+        <v>0</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R46" s="4">
+        <v>30</v>
+      </c>
       <c r="S46">
         <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:25">
       <c r="A47" s="1">
-        <v>46</v>
+        <v>934</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>35</v>
@@ -2863,13 +3397,25 @@
       <c r="K47" s="6">
         <v>448</v>
       </c>
+      <c r="L47" s="1">
+        <v>0</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R47" s="4">
+        <v>30</v>
+      </c>
       <c r="S47">
         <v>448</v>
       </c>
     </row>
     <row r="48" spans="1:25">
       <c r="A48" s="1">
-        <v>47</v>
+        <v>934</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>35</v>
@@ -2898,13 +3444,25 @@
       <c r="K48" s="6">
         <v>5930</v>
       </c>
+      <c r="L48" s="1">
+        <v>0</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R48" s="4">
+        <v>30</v>
+      </c>
       <c r="S48">
         <v>5930</v>
       </c>
     </row>
     <row r="49" spans="1:25">
       <c r="A49" s="1">
-        <v>48</v>
+        <v>934</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>35</v>
@@ -2933,13 +3491,25 @@
       <c r="K49" s="6">
         <v>440</v>
       </c>
+      <c r="L49" s="1">
+        <v>0</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R49" s="4">
+        <v>30</v>
+      </c>
       <c r="S49">
         <v>440</v>
       </c>
     </row>
     <row r="50" spans="1:25">
       <c r="A50" s="1">
-        <v>49</v>
+        <v>934</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>35</v>
@@ -2968,19 +3538,31 @@
       <c r="K50" s="6">
         <v>6920</v>
       </c>
+      <c r="L50" s="1">
+        <v>0</v>
+      </c>
       <c r="M50" s="6">
         <v>6565</v>
       </c>
       <c r="N50" t="s">
         <v>115</v>
       </c>
+      <c r="P50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R50" s="4">
+        <v>30</v>
+      </c>
       <c r="S50">
         <v>6920</v>
       </c>
     </row>
     <row r="51" spans="1:25">
       <c r="A51" s="1">
-        <v>50</v>
+        <v>934</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>35</v>
@@ -3009,19 +3591,31 @@
       <c r="K51" s="6">
         <v>5490</v>
       </c>
+      <c r="L51" s="1">
+        <v>0</v>
+      </c>
       <c r="M51" s="6">
         <v>1045</v>
       </c>
       <c r="N51" t="s">
         <v>115</v>
       </c>
+      <c r="P51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R51" s="4">
+        <v>30</v>
+      </c>
       <c r="S51">
         <v>5490</v>
       </c>
     </row>
     <row r="52" spans="1:25">
       <c r="A52" s="1">
-        <v>51</v>
+        <v>934</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>35</v>
@@ -3050,19 +3644,31 @@
       <c r="K52" s="6">
         <v>1269</v>
       </c>
+      <c r="L52" s="1">
+        <v>0</v>
+      </c>
       <c r="M52" s="6">
         <v>2539</v>
       </c>
       <c r="N52" t="s">
         <v>115</v>
       </c>
+      <c r="P52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R52" s="4">
+        <v>30</v>
+      </c>
       <c r="S52">
         <v>1269</v>
       </c>
     </row>
     <row r="53" spans="1:25">
       <c r="A53" s="1">
-        <v>52</v>
+        <v>934</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>35</v>
@@ -3091,19 +3697,31 @@
       <c r="K53" s="6">
         <v>15120</v>
       </c>
+      <c r="L53" s="1">
+        <v>0</v>
+      </c>
       <c r="M53" s="6">
         <v>840</v>
       </c>
       <c r="N53" t="s">
         <v>110</v>
       </c>
+      <c r="P53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R53" s="4">
+        <v>30</v>
+      </c>
       <c r="S53">
         <v>15120</v>
       </c>
     </row>
     <row r="54" spans="1:25">
       <c r="A54" s="1">
-        <v>53</v>
+        <v>934</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>35</v>
@@ -3132,19 +3750,31 @@
       <c r="K54" s="6">
         <v>180</v>
       </c>
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
       <c r="M54" s="6">
         <v>60</v>
       </c>
       <c r="N54" t="s">
         <v>114</v>
       </c>
+      <c r="P54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R54" s="4">
+        <v>30</v>
+      </c>
       <c r="S54">
         <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:25">
       <c r="A55" s="1">
-        <v>54</v>
+        <v>934</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>35</v>
@@ -3173,19 +3803,31 @@
       <c r="K55" s="6">
         <v>2850</v>
       </c>
+      <c r="L55" s="1">
+        <v>0</v>
+      </c>
       <c r="M55" s="6">
         <v>600</v>
       </c>
       <c r="N55" t="s">
         <v>115</v>
       </c>
+      <c r="P55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R55" s="4">
+        <v>30</v>
+      </c>
       <c r="S55">
         <v>2850</v>
       </c>
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="1">
-        <v>55</v>
+        <v>934</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>35</v>
@@ -3214,13 +3856,25 @@
       <c r="K56" s="6">
         <v>510</v>
       </c>
+      <c r="L56" s="1">
+        <v>0</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R56" s="4">
+        <v>30</v>
+      </c>
       <c r="S56">
         <v>510</v>
       </c>
     </row>
     <row r="57" spans="1:25">
       <c r="A57" s="1">
-        <v>56</v>
+        <v>934</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>35</v>
@@ -3249,13 +3903,25 @@
       <c r="K57" s="6">
         <v>387</v>
       </c>
+      <c r="L57" s="1">
+        <v>0</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R57" s="4">
+        <v>30</v>
+      </c>
       <c r="S57">
         <v>387</v>
       </c>
     </row>
     <row r="58" spans="1:25">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>934</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>35</v>
@@ -3284,16 +3950,28 @@
       <c r="K58" s="6">
         <v>69469</v>
       </c>
+      <c r="L58" s="1">
+        <v>0</v>
+      </c>
       <c r="M58" s="6">
         <v>443125</v>
       </c>
       <c r="N58" t="s">
         <v>115</v>
       </c>
+      <c r="P58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R58" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="59" spans="1:25">
       <c r="A59" s="1">
-        <v>56</v>
+        <v>934</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>35</v>
@@ -3322,16 +4000,28 @@
       <c r="K59" s="6">
         <v>281</v>
       </c>
+      <c r="L59" s="1">
+        <v>0</v>
+      </c>
       <c r="M59" s="6">
         <v>1875</v>
       </c>
       <c r="N59" t="s">
         <v>115</v>
       </c>
+      <c r="P59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R59" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="60" spans="1:25">
       <c r="A60" s="1">
-        <v>56</v>
+        <v>934</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>35</v>
@@ -3360,16 +4050,28 @@
       <c r="K60" s="6">
         <v>16882</v>
       </c>
+      <c r="L60" s="1">
+        <v>0</v>
+      </c>
       <c r="M60" s="6">
         <v>114550</v>
       </c>
       <c r="N60" t="s">
         <v>115</v>
       </c>
+      <c r="P60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R60" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="61" spans="1:25">
       <c r="A61" s="1">
-        <v>56</v>
+        <v>934</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>35</v>
@@ -3398,16 +4100,28 @@
       <c r="K61" s="6">
         <v>72523</v>
       </c>
+      <c r="L61" s="1">
+        <v>0</v>
+      </c>
       <c r="M61" s="6">
         <v>483488</v>
       </c>
       <c r="N61" t="s">
         <v>115</v>
       </c>
+      <c r="P61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R61" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="62" spans="1:25">
       <c r="A62" s="1">
-        <v>57</v>
+        <v>934</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>35</v>
@@ -3437,20 +4151,31 @@
       <c r="K62" s="18">
         <v>20407</v>
       </c>
-      <c r="L62" s="17"/>
+      <c r="L62" s="1">
+        <v>0</v>
+      </c>
       <c r="M62" s="18">
         <v>136050</v>
       </c>
       <c r="N62" s="19" t="s">
         <v>115</v>
       </c>
+      <c r="P62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R62" s="4">
+        <v>30</v>
+      </c>
       <c r="Y62" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:25">
       <c r="A63" s="1">
-        <v>58</v>
+        <v>934</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>35</v>
@@ -3480,20 +4205,31 @@
       <c r="K63" s="16">
         <v>15446</v>
       </c>
-      <c r="L63" s="15"/>
+      <c r="L63" s="1">
+        <v>0</v>
+      </c>
       <c r="M63" s="16">
         <v>102975</v>
       </c>
       <c r="N63" t="s">
         <v>115</v>
       </c>
+      <c r="P63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R63" s="4">
+        <v>30</v>
+      </c>
       <c r="S63">
         <v>15446</v>
       </c>
     </row>
     <row r="64" spans="1:25">
       <c r="A64" s="1">
-        <v>59</v>
+        <v>934</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>35</v>
@@ -3522,16 +4258,28 @@
       <c r="K64">
         <v>5770</v>
       </c>
+      <c r="L64" s="1">
+        <v>0</v>
+      </c>
       <c r="M64" s="6">
         <v>144.25</v>
       </c>
       <c r="N64" s="7" t="s">
         <v>140</v>
       </c>
+      <c r="P64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R64" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="65" spans="1:25">
       <c r="A65" s="1">
-        <v>60</v>
+        <v>934</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>35</v>
@@ -3560,19 +4308,31 @@
       <c r="K65">
         <v>124975</v>
       </c>
+      <c r="L65" s="1">
+        <v>0</v>
+      </c>
       <c r="M65" s="6">
         <v>24995</v>
       </c>
       <c r="N65" t="s">
         <v>115</v>
       </c>
+      <c r="P65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R65" s="4">
+        <v>30</v>
+      </c>
       <c r="S65">
         <v>124975</v>
       </c>
     </row>
     <row r="66" spans="1:25">
       <c r="A66" s="1">
-        <v>61</v>
+        <v>934</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>35</v>
@@ -3601,19 +4361,31 @@
       <c r="K66">
         <v>2160</v>
       </c>
+      <c r="L66" s="1">
+        <v>0</v>
+      </c>
       <c r="M66" s="6">
         <v>540</v>
       </c>
       <c r="N66" t="s">
         <v>116</v>
       </c>
+      <c r="P66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R66" s="4">
+        <v>30</v>
+      </c>
       <c r="S66">
         <v>2160</v>
       </c>
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="1">
-        <v>62</v>
+        <v>934</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>35</v>
@@ -3642,19 +4414,31 @@
       <c r="K67">
         <v>16995</v>
       </c>
+      <c r="L67" s="1">
+        <v>0</v>
+      </c>
       <c r="M67" s="6">
         <v>3090</v>
       </c>
       <c r="N67" t="s">
         <v>116</v>
       </c>
+      <c r="P67" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R67" s="4">
+        <v>30</v>
+      </c>
       <c r="S67">
         <v>16995</v>
       </c>
     </row>
     <row r="68" spans="1:25">
       <c r="A68" s="1">
-        <v>63</v>
+        <v>934</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>35</v>
@@ -3683,19 +4467,31 @@
       <c r="K68">
         <v>25800</v>
       </c>
+      <c r="L68" s="1">
+        <v>0</v>
+      </c>
       <c r="M68" s="6">
         <v>5160</v>
       </c>
       <c r="N68" t="s">
         <v>116</v>
       </c>
+      <c r="P68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q68" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R68" s="4">
+        <v>30</v>
+      </c>
       <c r="S68">
         <v>25800</v>
       </c>
     </row>
     <row r="69" spans="1:25">
       <c r="A69" s="1">
-        <v>64</v>
+        <v>934</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>35</v>
@@ -3724,19 +4520,31 @@
       <c r="K69">
         <v>160</v>
       </c>
+      <c r="L69" s="1">
+        <v>0</v>
+      </c>
       <c r="M69" s="6">
         <v>80</v>
       </c>
       <c r="N69" t="s">
         <v>116</v>
       </c>
+      <c r="P69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q69" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R69" s="4">
+        <v>30</v>
+      </c>
       <c r="S69">
         <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:25">
       <c r="A70" s="1">
-        <v>65</v>
+        <v>934</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>35</v>
@@ -3765,19 +4573,31 @@
       <c r="K70">
         <v>3900</v>
       </c>
+      <c r="L70" s="1">
+        <v>0</v>
+      </c>
       <c r="M70" s="6">
         <v>650</v>
       </c>
       <c r="N70" t="s">
         <v>116</v>
       </c>
+      <c r="P70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R70" s="4">
+        <v>30</v>
+      </c>
       <c r="S70">
         <v>3900</v>
       </c>
     </row>
     <row r="71" spans="1:25">
       <c r="A71" s="1">
-        <v>66</v>
+        <v>934</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>35</v>
@@ -3806,19 +4626,31 @@
       <c r="K71">
         <v>2160</v>
       </c>
+      <c r="L71" s="1">
+        <v>0</v>
+      </c>
       <c r="M71" s="6">
         <v>360</v>
       </c>
       <c r="N71" t="s">
         <v>116</v>
       </c>
+      <c r="P71" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R71" s="4">
+        <v>30</v>
+      </c>
       <c r="S71">
         <v>2160</v>
       </c>
     </row>
     <row r="72" spans="1:25">
       <c r="A72" s="1">
-        <v>67</v>
+        <v>934</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>35</v>
@@ -3847,19 +4679,31 @@
       <c r="K72">
         <v>5208</v>
       </c>
+      <c r="L72" s="1">
+        <v>0</v>
+      </c>
       <c r="M72" s="6">
         <v>868</v>
       </c>
       <c r="N72" t="s">
         <v>116</v>
       </c>
+      <c r="P72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R72" s="4">
+        <v>30</v>
+      </c>
       <c r="S72">
         <v>5208</v>
       </c>
     </row>
     <row r="73" spans="1:25">
       <c r="A73" s="1">
-        <v>68</v>
+        <v>934</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>35</v>
@@ -3888,13 +4732,25 @@
       <c r="K73">
         <v>6370</v>
       </c>
+      <c r="L73" s="1">
+        <v>0</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R73" s="4">
+        <v>30</v>
+      </c>
       <c r="S73">
         <v>6370</v>
       </c>
     </row>
     <row r="74" spans="1:25">
       <c r="A74" s="1">
-        <v>69</v>
+        <v>934</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>35</v>
@@ -3923,19 +4779,31 @@
       <c r="K74">
         <v>234</v>
       </c>
+      <c r="L74" s="1">
+        <v>0</v>
+      </c>
       <c r="M74" s="6">
         <v>937</v>
       </c>
       <c r="N74" t="s">
         <v>114</v>
       </c>
+      <c r="P74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R74" s="4">
+        <v>30</v>
+      </c>
       <c r="S74">
         <v>234</v>
       </c>
     </row>
     <row r="75" spans="1:25">
       <c r="A75" s="1">
-        <v>70</v>
+        <v>934</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>35</v>
@@ -3963,6 +4831,9 @@
       </c>
       <c r="K75">
         <v>450</v>
+      </c>
+      <c r="L75" s="1">
+        <v>0</v>
       </c>
       <c r="M75" s="8">
         <f>3+(37/288)</f>
@@ -3971,6 +4842,15 @@
       <c r="N75" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="P75" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R75" s="4">
+        <v>30</v>
+      </c>
       <c r="S75">
         <v>450</v>
       </c>
@@ -3980,7 +4860,7 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="1">
-        <v>71</v>
+        <v>934</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>35</v>
@@ -4009,19 +4889,31 @@
       <c r="K76">
         <v>528</v>
       </c>
+      <c r="L76" s="1">
+        <v>0</v>
+      </c>
       <c r="M76" s="6">
         <v>264</v>
       </c>
       <c r="N76" t="s">
         <v>112</v>
       </c>
+      <c r="P76" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R76" s="4">
+        <v>30</v>
+      </c>
       <c r="S76">
         <v>528</v>
       </c>
     </row>
     <row r="77" spans="1:25">
       <c r="A77" s="1">
-        <v>72</v>
+        <v>934</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>35</v>
@@ -4050,11 +4942,24 @@
       <c r="K77">
         <v>260</v>
       </c>
+      <c r="L77" s="1">
+        <v>0</v>
+      </c>
+      <c r="P77" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R77" s="4">
+        <v>30</v>
+      </c>
       <c r="S77">
         <v>260</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>